<commit_message>
et: Addn CES files
</commit_message>
<xml_diff>
--- a/Coverage Survey/Ethiopia/et_ces_sch_sth_1_village_202111.xlsx
+++ b/Coverage Survey/Ethiopia/et_ces_sch_sth_1_village_202111.xlsx
@@ -84,7 +84,7 @@
     <t>3. GPS North on Arrival</t>
   </si>
   <si>
-    <t>select_ont woreda</t>
+    <t>select_one woreda</t>
   </si>
   <si>
     <t>v_woreda</t>
@@ -114,28 +114,28 @@
     <t>6. What is the position in the village of the person being interviewed?</t>
   </si>
   <si>
+    <t>v_population</t>
+  </si>
+  <si>
+    <t>7. What is the total population of the village?</t>
+  </si>
+  <si>
+    <t>v_hh_number</t>
+  </si>
+  <si>
+    <t>8. What is the number of households in the village (interviewee to estimate if not known)</t>
+  </si>
+  <si>
+    <t>select_one data_source</t>
+  </si>
+  <si>
+    <t>v_src_data</t>
+  </si>
+  <si>
+    <t>9. Source of population data?</t>
+  </si>
+  <si>
     <t>text</t>
-  </si>
-  <si>
-    <t>v_population</t>
-  </si>
-  <si>
-    <t>7. What is the total population of the village?</t>
-  </si>
-  <si>
-    <t>v_hh_number</t>
-  </si>
-  <si>
-    <t>8. What is the number of households in the village (interviewee to estimate if not known)</t>
-  </si>
-  <si>
-    <t>select_one data_source</t>
-  </si>
-  <si>
-    <t>v_src_data</t>
-  </si>
-  <si>
-    <t>9. Source of population data?</t>
   </si>
   <si>
     <t>v_src_data_other</t>
@@ -1385,10 +1385,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1414,11 +1414,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1426,6 +1425,28 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1438,30 +1459,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1476,25 +1474,17 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1506,22 +1496,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1536,14 +1520,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1552,6 +1529,29 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1586,7 +1586,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1598,19 +1628,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1622,7 +1646,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1634,7 +1658,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1646,25 +1706,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1682,85 +1760,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1774,50 +1774,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1840,8 +1801,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1853,6 +1829,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1871,155 +1856,170 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2038,7 +2038,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -2365,7 +2364,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D$1:D$1048576"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.425" defaultRowHeight="12.75"/>
@@ -2399,22 +2398,22 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2492,12 +2491,12 @@
       <c r="E6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="13"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="8"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="13" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2517,13 +2516,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>14</v>
@@ -2534,10 +2533,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>36</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>14</v>
@@ -2545,13 +2544,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>39</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>14</v>
@@ -2559,7 +2558,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>40</v>
@@ -2810,7 +2809,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
et: ces Wondows update
</commit_message>
<xml_diff>
--- a/Coverage Survey/Ethiopia/et_ces_sch_sth_1_village_202111.xlsx
+++ b/Coverage Survey/Ethiopia/et_ces_sch_sth_1_village_202111.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\Coverage Survey\Ethiopia\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EBADCC-4C3E-4FDF-8C06-01F2BF19762F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12345"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="144525" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -1383,14 +1389,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1413,159 +1413,8 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1578,194 +1427,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1773,251 +1436,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2041,61 +1462,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2353,36 +1730,37 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.425" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
   <cols>
-    <col min="1" max="1" width="19.7083333333333" customWidth="1"/>
+    <col min="1" max="1" width="19.703125" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="45.875" customWidth="1"/>
-    <col min="4" max="4" width="25.2833333333333" customWidth="1"/>
+    <col min="3" max="3" width="45.87890625" customWidth="1"/>
+    <col min="4" max="4" width="25.29296875" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="16.2833333333333" customWidth="1"/>
-    <col min="7" max="7" width="28.5666666666667" customWidth="1"/>
-    <col min="8" max="8" width="12.375" customWidth="1"/>
-    <col min="9" max="9" width="22.25" customWidth="1"/>
-    <col min="10" max="10" width="11.375" customWidth="1"/>
-    <col min="11" max="11" width="16.7083333333333" customWidth="1"/>
+    <col min="6" max="6" width="16.29296875" customWidth="1"/>
+    <col min="7" max="7" width="28.5859375" customWidth="1"/>
+    <col min="8" max="8" width="12.3515625" customWidth="1"/>
+    <col min="9" max="9" width="22.234375" customWidth="1"/>
+    <col min="10" max="10" width="11.3515625" customWidth="1"/>
+    <col min="11" max="11" width="16.703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:11">
+    <row r="1" spans="1:11" s="6" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2417,7 +1795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:11">
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
@@ -2432,7 +1810,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:11">
       <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
@@ -2450,7 +1828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:11">
       <c r="A4" s="8" t="s">
         <v>19</v>
       </c>
@@ -2464,7 +1842,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:11">
       <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
@@ -2478,7 +1856,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" s="7" customFormat="1" spans="1:11">
+    <row r="6" spans="1:11" s="7" customFormat="1">
       <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
@@ -2500,7 +1878,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" ht="25.5" spans="1:5">
+    <row r="7" spans="1:11" ht="25.35">
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
@@ -2514,7 +1892,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:11">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
@@ -2528,7 +1906,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" ht="25.5" spans="1:5">
+    <row r="9" spans="1:11" ht="25.35">
       <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
@@ -2542,7 +1920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2556,7 +1934,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2574,7 +1952,7 @@
       </c>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" ht="25.5" spans="1:8">
+    <row r="12" spans="1:11" ht="25.35">
       <c r="A12" s="8" t="s">
         <v>43</v>
       </c>
@@ -2591,7 +1969,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" ht="25.5" spans="1:6">
+    <row r="13" spans="1:11">
       <c r="A13" s="8" t="s">
         <v>47</v>
       </c>
@@ -2606,7 +1984,7 @@
       </c>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:11">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
@@ -2626,7 +2004,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:11">
       <c r="A15" s="11" t="s">
         <v>54</v>
       </c>
@@ -2637,7 +2015,7 @@
       </c>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="11" t="s">
         <v>55</v>
       </c>
@@ -2653,7 +2031,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" ht="25.5" spans="1:5">
+    <row r="17" spans="1:5" ht="25.35">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -2667,7 +2045,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" ht="25.5" spans="1:5">
+    <row r="18" spans="1:5" ht="25.35">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -2681,7 +2059,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" ht="38.25" spans="1:5">
+    <row r="19" spans="1:5" ht="38">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -2695,7 +2073,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" ht="38.25" spans="1:5">
+    <row r="20" spans="1:5" ht="38">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -2723,7 +2101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" ht="25.5" spans="1:5">
+    <row r="22" spans="1:5" ht="25.35">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -2807,7 +2185,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -2818,7 +2196,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -2826,7 +2204,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -2846,7 +2224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2854,19 +2232,18 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A315" activePane="bottomLeft" state="frozen"/>
-      <selection/>
       <selection pane="bottomLeft" activeCell="A347" sqref="A347:A358"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.425" defaultRowHeight="12.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
   <cols>
-    <col min="1" max="1" width="11.425" customWidth="1"/>
-    <col min="2" max="3" width="19.8583333333333" customWidth="1"/>
-    <col min="4" max="4" width="13.2833333333333" customWidth="1"/>
+    <col min="1" max="1" width="11.41015625" customWidth="1"/>
+    <col min="2" max="3" width="19.87890625" customWidth="1"/>
+    <col min="4" max="4" width="13.29296875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" spans="1:6">
+    <row r="1" spans="1:6" s="3" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>91</v>
       </c>
@@ -2882,7 +2259,7 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -2893,7 +2270,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -2904,7 +2281,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -2915,7 +2292,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -2926,7 +2303,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -2937,7 +2314,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -2948,7 +2325,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -2959,7 +2336,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>92</v>
       </c>
@@ -2970,7 +2347,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>92</v>
       </c>
@@ -2981,7 +2358,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -2992,7 +2369,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -3006,7 +2383,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -3020,7 +2397,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -3034,7 +2411,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>103</v>
       </c>
@@ -7192,7 +6569,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="314" spans="1:3">
+    <row r="314" spans="1:4">
       <c r="A314" s="5" t="s">
         <v>404</v>
       </c>
@@ -7203,7 +6580,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:4">
       <c r="A315" s="5" t="s">
         <v>404</v>
       </c>
@@ -7214,7 +6591,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="316" spans="1:3">
+    <row r="316" spans="1:4">
       <c r="A316" s="5" t="s">
         <v>404</v>
       </c>
@@ -7225,7 +6602,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="318" spans="1:3">
+    <row r="318" spans="1:4">
       <c r="A318" t="s">
         <v>408</v>
       </c>
@@ -7236,7 +6613,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="319" spans="1:3">
+    <row r="319" spans="1:4">
       <c r="A319" t="s">
         <v>408</v>
       </c>
@@ -7247,7 +6624,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="320" spans="1:3">
+    <row r="320" spans="1:4">
       <c r="A320" t="s">
         <v>408</v>
       </c>
@@ -7633,7 +7010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -7643,13 +7020,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.425" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="11.41015625" defaultRowHeight="12.7"/>
   <cols>
     <col min="1" max="1" width="55" customWidth="1"/>
-    <col min="2" max="2" width="45.425" customWidth="1"/>
+    <col min="2" max="2" width="45.41015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>448</v>
       </c>

</xml_diff>